<commit_message>
logistic regression does not fit
</commit_message>
<xml_diff>
--- a/output/fit-models.xlsx
+++ b/output/fit-models.xlsx
@@ -439,7 +439,7 @@
         </is>
       </c>
       <c r="B2">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C2">
         <v>0.096</v>
@@ -448,62 +448,62 @@
         <v>0.002</v>
       </c>
       <c r="E2">
-        <v>4.962</v>
+        <v>11.486</v>
       </c>
       <c r="F2">
-        <v>1.549</v>
+        <v>3.522</v>
       </c>
       <c r="G2">
-        <v>3.205</v>
+        <v>3.262</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>0.047</v>
       </c>
       <c r="I2">
-        <v>51.527</v>
+        <v>25.703</v>
       </c>
       <c r="J2">
-        <v>5.086</v>
+        <v>12.759</v>
       </c>
       <c r="K2">
-        <v>10.13</v>
+        <v>2.014</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>unemployment_rate</t>
+          <t>indulgence</t>
         </is>
       </c>
       <c r="B3">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="C3">
-        <v>0.085</v>
+        <v>0.041</v>
       </c>
       <c r="D3">
-        <v>0.022</v>
+        <v>0.069</v>
       </c>
       <c r="E3">
-        <v>1.094</v>
+        <v>9.223</v>
       </c>
       <c r="F3">
-        <v>0.466</v>
+        <v>4.995</v>
       </c>
       <c r="G3">
-        <v>2.346</v>
+        <v>1.847</v>
       </c>
       <c r="H3">
-        <v>0.106</v>
+        <v>0.57</v>
       </c>
       <c r="I3">
-        <v>2.712</v>
+        <v>10.485</v>
       </c>
       <c r="J3">
-        <v>1.65</v>
+        <v>18.364</v>
       </c>
       <c r="K3">
-        <v>1.644</v>
+        <v>0.571</v>
       </c>
     </row>
     <row r="4">
@@ -513,182 +513,182 @@
         </is>
       </c>
       <c r="B4">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C4">
-        <v>0.041</v>
+        <v>0.024</v>
       </c>
       <c r="D4">
-        <v>0.044</v>
+        <v>0.119</v>
       </c>
       <c r="E4">
-        <v>3.505</v>
+        <v>6.236</v>
       </c>
       <c r="F4">
-        <v>1.718</v>
+        <v>3.966</v>
       </c>
       <c r="G4">
-        <v>2.04</v>
+        <v>1.572</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>0.226</v>
       </c>
       <c r="I4">
-        <v>29.137</v>
+        <v>17.499</v>
       </c>
       <c r="J4">
-        <v>5.644</v>
+        <v>14.368</v>
       </c>
       <c r="K4">
-        <v>5.162</v>
+        <v>1.218</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>indulgence</t>
+          <t>power_distance</t>
         </is>
       </c>
       <c r="B5">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="C5">
-        <v>0.025</v>
+        <v>0.024</v>
       </c>
       <c r="D5">
-        <v>0.165</v>
+        <v>0.121</v>
       </c>
       <c r="E5">
-        <v>2.799</v>
+        <v>-5.742</v>
       </c>
       <c r="F5">
-        <v>1.995</v>
+        <v>3.674</v>
       </c>
       <c r="G5">
-        <v>1.403</v>
+        <v>-1.563</v>
       </c>
       <c r="H5">
         <v>0</v>
       </c>
       <c r="I5">
-        <v>35.347</v>
+        <v>87.39</v>
       </c>
       <c r="J5">
-        <v>6.725</v>
+        <v>13.313</v>
       </c>
       <c r="K5">
-        <v>5.256</v>
+        <v>6.564</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>power_distance</t>
+          <t>democracy</t>
         </is>
       </c>
       <c r="B6">
-        <v>95</v>
+        <v>139</v>
       </c>
       <c r="C6">
-        <v>0.017</v>
+        <v>0.011</v>
       </c>
       <c r="D6">
-        <v>0.198</v>
+        <v>0.209</v>
       </c>
       <c r="E6">
-        <v>-2.068</v>
+        <v>0.417</v>
       </c>
       <c r="F6">
-        <v>1.595</v>
+        <v>0.331</v>
       </c>
       <c r="G6">
-        <v>-1.296</v>
+        <v>1.261</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="I6">
-        <v>72.862</v>
+        <v>3.854</v>
       </c>
       <c r="J6">
-        <v>5.24</v>
+        <v>1.194</v>
       </c>
       <c r="K6">
-        <v>13.906</v>
+        <v>3.229</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>motivation</t>
+          <t>masculinity</t>
         </is>
       </c>
       <c r="B7">
-        <v>95</v>
+        <v>55</v>
       </c>
       <c r="C7">
-        <v>0.015</v>
+        <v>0.028</v>
       </c>
       <c r="D7">
-        <v>0.222</v>
+        <v>0.22</v>
       </c>
       <c r="E7">
-        <v>-1.678</v>
+        <v>-5.332</v>
       </c>
       <c r="F7">
-        <v>1.365</v>
+        <v>4.3</v>
       </c>
       <c r="G7">
-        <v>-1.229</v>
+        <v>-1.24</v>
       </c>
       <c r="H7">
         <v>0</v>
       </c>
       <c r="I7">
-        <v>51.908</v>
+        <v>69.316</v>
       </c>
       <c r="J7">
-        <v>4.482</v>
+        <v>15.374</v>
       </c>
       <c r="K7">
-        <v>11.581</v>
+        <v>4.509</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>masculinity</t>
+          <t>unemployment_rate</t>
         </is>
       </c>
       <c r="B8">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="C8">
-        <v>0.025</v>
+        <v>0.023</v>
       </c>
       <c r="D8">
-        <v>0.26</v>
+        <v>0.237</v>
       </c>
       <c r="E8">
-        <v>-1.962</v>
+        <v>1.346</v>
       </c>
       <c r="F8">
-        <v>1.723</v>
+        <v>1.126</v>
       </c>
       <c r="G8">
-        <v>-1.139</v>
+        <v>1.195</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>0.703</v>
       </c>
       <c r="I8">
-        <v>55.628</v>
+        <v>1.615</v>
       </c>
       <c r="J8">
-        <v>5.464</v>
+        <v>4.212</v>
       </c>
       <c r="K8">
-        <v>10.181</v>
+        <v>0.383</v>
       </c>
     </row>
     <row r="9">
@@ -698,182 +698,182 @@
         </is>
       </c>
       <c r="B9">
-        <v>152</v>
+        <v>163</v>
       </c>
       <c r="C9">
-        <v>0.006</v>
+        <v>0.007</v>
       </c>
       <c r="D9">
-        <v>0.304</v>
+        <v>0.272</v>
       </c>
       <c r="E9">
-        <v>1.786</v>
+        <v>4.164</v>
       </c>
       <c r="F9">
-        <v>1.731</v>
+        <v>3.781</v>
       </c>
       <c r="G9">
-        <v>1.032</v>
+        <v>1.101</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="I9">
-        <v>53.771</v>
+        <v>44.43</v>
       </c>
       <c r="J9">
-        <v>5.534</v>
+        <v>13.471</v>
       </c>
       <c r="K9">
-        <v>9.717</v>
+        <v>3.298</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>mean_years_of_schooling</t>
+          <t>expected_years_of_schooling</t>
         </is>
       </c>
       <c r="B10">
-        <v>153</v>
+        <v>164</v>
       </c>
       <c r="C10">
-        <v>0.006</v>
+        <v>0.004</v>
       </c>
       <c r="D10">
-        <v>0.335</v>
+        <v>0.381</v>
       </c>
       <c r="E10">
-        <v>-0.179</v>
+        <v>0.317</v>
       </c>
       <c r="F10">
-        <v>0.185</v>
+        <v>0.361</v>
       </c>
       <c r="G10">
-        <v>-0.966</v>
+        <v>0.878</v>
       </c>
       <c r="H10">
         <v>0</v>
       </c>
       <c r="I10">
-        <v>9.444</v>
+        <v>12.37</v>
       </c>
       <c r="J10">
-        <v>0.589</v>
+        <v>1.283</v>
       </c>
       <c r="K10">
-        <v>16.036</v>
+        <v>9.638</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>life_expectancy</t>
+          <t>motivation</t>
         </is>
       </c>
       <c r="B11">
-        <v>154</v>
+        <v>98</v>
       </c>
       <c r="C11">
-        <v>0.003</v>
+        <v>0.004</v>
       </c>
       <c r="D11">
-        <v>0.462</v>
+        <v>0.523</v>
       </c>
       <c r="E11">
-        <v>-0.323</v>
+        <v>-1.996</v>
       </c>
       <c r="F11">
-        <v>0.438</v>
+        <v>3.113</v>
       </c>
       <c r="G11">
-        <v>-0.737</v>
+        <v>-0.641</v>
       </c>
       <c r="H11">
         <v>0</v>
       </c>
       <c r="I11">
-        <v>72.339</v>
+        <v>54.222</v>
       </c>
       <c r="J11">
-        <v>1.391</v>
+        <v>11.279</v>
       </c>
       <c r="K11">
-        <v>51.995</v>
+        <v>4.808</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>human_development_index</t>
+          <t>mean_years_of_schooling</t>
         </is>
       </c>
       <c r="B12">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="C12">
-        <v>0.003</v>
+        <v>0.002</v>
       </c>
       <c r="D12">
-        <v>0.471</v>
+        <v>0.588</v>
       </c>
       <c r="E12">
-        <v>-0.006</v>
+        <v>-0.217</v>
       </c>
       <c r="F12">
-        <v>0.009</v>
+        <v>0.4</v>
       </c>
       <c r="G12">
-        <v>-0.722</v>
+        <v>-0.542</v>
       </c>
       <c r="H12">
         <v>0</v>
       </c>
       <c r="I12">
-        <v>0.739</v>
+        <v>9.678</v>
       </c>
       <c r="J12">
-        <v>0.028</v>
+        <v>1.423</v>
       </c>
       <c r="K12">
-        <v>26.643</v>
+        <v>6.799</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>democracy</t>
+          <t>gdp_per_capita</t>
         </is>
       </c>
       <c r="B13">
-        <v>132</v>
+        <v>165</v>
       </c>
       <c r="C13">
-        <v>0.003</v>
+        <v>0.001</v>
       </c>
       <c r="D13">
-        <v>0.525</v>
+        <v>0.643</v>
       </c>
       <c r="E13">
-        <v>0.096</v>
+        <v>0.097</v>
       </c>
       <c r="F13">
-        <v>0.15</v>
+        <v>0.209</v>
       </c>
       <c r="G13">
-        <v>0.638</v>
+        <v>0.464</v>
       </c>
       <c r="H13">
         <v>0</v>
       </c>
       <c r="I13">
-        <v>5.085</v>
+        <v>8.448</v>
       </c>
       <c r="J13">
-        <v>0.492</v>
+        <v>0.746</v>
       </c>
       <c r="K13">
-        <v>10.327</v>
+        <v>11.319</v>
       </c>
     </row>
     <row r="14">
@@ -883,219 +883,219 @@
         </is>
       </c>
       <c r="B14">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="C14">
         <v>0.001</v>
       </c>
       <c r="D14">
-        <v>0.697</v>
+        <v>0.648</v>
       </c>
       <c r="E14">
-        <v>-0.43</v>
+        <v>-1.09</v>
       </c>
       <c r="F14">
-        <v>1.103</v>
+        <v>2.386</v>
       </c>
       <c r="G14">
-        <v>-0.39</v>
+        <v>-0.457</v>
       </c>
       <c r="H14">
         <v>0</v>
       </c>
       <c r="I14">
-        <v>44.431</v>
+        <v>46.904</v>
       </c>
       <c r="J14">
-        <v>3.559</v>
+        <v>8.549</v>
       </c>
       <c r="K14">
-        <v>12.484</v>
+        <v>5.487</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>long_term_orientation</t>
+          <t>safety_index</t>
         </is>
       </c>
       <c r="B15">
-        <v>86</v>
+        <v>116</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="D15">
-        <v>0.873</v>
+        <v>0.678</v>
       </c>
       <c r="E15">
-        <v>-0.255</v>
+        <v>-1.105</v>
       </c>
       <c r="F15">
-        <v>1.595</v>
+        <v>2.651</v>
       </c>
       <c r="G15">
-        <v>-0.16</v>
+        <v>-0.417</v>
       </c>
       <c r="H15">
         <v>0</v>
       </c>
       <c r="I15">
-        <v>40.051</v>
+        <v>58.798</v>
       </c>
       <c r="J15">
-        <v>5.318</v>
+        <v>9.528</v>
       </c>
       <c r="K15">
-        <v>7.531</v>
+        <v>6.171</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>gdp_per_capita</t>
+          <t>crime_index</t>
         </is>
       </c>
       <c r="B16">
-        <v>154</v>
+        <v>116</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="D16">
-        <v>0.89</v>
+        <v>0.678</v>
       </c>
       <c r="E16">
-        <v>-0.012</v>
+        <v>1.105</v>
       </c>
       <c r="F16">
-        <v>0.086</v>
+        <v>2.651</v>
       </c>
       <c r="G16">
-        <v>-0.138</v>
+        <v>0.417</v>
       </c>
       <c r="H16">
         <v>0</v>
       </c>
       <c r="I16">
-        <v>8.823</v>
+        <v>41.202</v>
       </c>
       <c r="J16">
-        <v>0.273</v>
+        <v>9.528</v>
       </c>
       <c r="K16">
-        <v>32.378</v>
+        <v>4.324</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>safety_index</t>
+          <t>long_term_orientation</t>
         </is>
       </c>
       <c r="B17">
-        <v>111</v>
+        <v>89</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="D17">
-        <v>0.893</v>
+        <v>0.805</v>
       </c>
       <c r="E17">
-        <v>-0.138</v>
+        <v>0.995</v>
       </c>
       <c r="F17">
-        <v>1.026</v>
+        <v>4.018</v>
       </c>
       <c r="G17">
-        <v>-0.134</v>
+        <v>0.248</v>
       </c>
       <c r="H17">
-        <v>0</v>
+        <v>0.018</v>
       </c>
       <c r="I17">
-        <v>55.054</v>
+        <v>35.299</v>
       </c>
       <c r="J17">
-        <v>3.279</v>
+        <v>14.685</v>
       </c>
       <c r="K17">
-        <v>16.791</v>
+        <v>2.404</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>crime_index</t>
+          <t>human_development_index</t>
         </is>
       </c>
       <c r="B18">
-        <v>111</v>
+        <v>163</v>
       </c>
       <c r="C18">
         <v>0</v>
       </c>
       <c r="D18">
-        <v>0.893</v>
+        <v>0.985</v>
       </c>
       <c r="E18">
-        <v>0.138</v>
+        <v>0</v>
       </c>
       <c r="F18">
-        <v>1.026</v>
+        <v>0.019</v>
       </c>
       <c r="G18">
-        <v>0.134</v>
+        <v>0.019</v>
       </c>
       <c r="H18">
         <v>0</v>
       </c>
       <c r="I18">
-        <v>44.946</v>
+        <v>0.717</v>
       </c>
       <c r="J18">
-        <v>3.279</v>
+        <v>0.067</v>
       </c>
       <c r="K18">
-        <v>13.708</v>
+        <v>10.651</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>expected_years_of_schooling</t>
+          <t>life_expectancy</t>
         </is>
       </c>
       <c r="B19">
-        <v>153</v>
+        <v>165</v>
       </c>
       <c r="C19">
         <v>0</v>
       </c>
       <c r="D19">
-        <v>0.897</v>
+        <v>0.99</v>
       </c>
       <c r="E19">
-        <v>0.022</v>
+        <v>-0.012</v>
       </c>
       <c r="F19">
-        <v>0.167</v>
+        <v>0.972</v>
       </c>
       <c r="G19">
-        <v>0.13</v>
+        <v>-0.012</v>
       </c>
       <c r="H19">
         <v>0</v>
       </c>
       <c r="I19">
-        <v>13.517</v>
+        <v>71.167</v>
       </c>
       <c r="J19">
-        <v>0.532</v>
+        <v>3.458</v>
       </c>
       <c r="K19">
-        <v>25.412</v>
+        <v>20.582</v>
       </c>
     </row>
   </sheetData>

</xml_diff>